<commit_message>
BC Mgmt and Agg Done Agent Pending
</commit_message>
<xml_diff>
--- a/src/main/java/SOR_resources/Test_Data.xlsx
+++ b/src/main/java/SOR_resources/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24345" windowHeight="11850" activeTab="2"/>
+    <workbookView windowWidth="24345" windowHeight="11505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CV_LoginTestCase" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="161">
   <si>
     <t>Module</t>
   </si>
@@ -434,6 +434,84 @@
   </si>
   <si>
     <t>Switch_Percentage</t>
+  </si>
+  <si>
+    <t>BC_Registration</t>
+  </si>
+  <si>
+    <t>BC_Name</t>
+  </si>
+  <si>
+    <t>MaximusInfoNew</t>
+  </si>
+  <si>
+    <t>PanNo</t>
+  </si>
+  <si>
+    <t>QXOPC5696Y</t>
+  </si>
+  <si>
+    <t>AddharNO</t>
+  </si>
+  <si>
+    <t>502081483187</t>
+  </si>
+  <si>
+    <t>AccountNo</t>
+  </si>
+  <si>
+    <t>IFSCcode</t>
+  </si>
+  <si>
+    <t>HDFC0000967</t>
+  </si>
+  <si>
+    <t>Addess</t>
+  </si>
+  <si>
+    <t>Thane Maharshtra</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Sangli</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Satna</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>abc12356@abc.com</t>
+  </si>
+  <si>
+    <t>ContactNo</t>
+  </si>
+  <si>
+    <t>AGG_Registration</t>
+  </si>
+  <si>
+    <t>AGG_Name</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>12th</t>
   </si>
 </sst>
 </file>
@@ -1090,6 +1168,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2615,10 +2694,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2628,51 +2707,98 @@
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="18.625" customWidth="1"/>
     <col min="5" max="5" width="18.125" customWidth="1"/>
-    <col min="6" max="6" width="28.75" customWidth="1"/>
+    <col min="6" max="6" width="26.625" customWidth="1"/>
     <col min="7" max="7" width="14.375" customWidth="1"/>
+    <col min="8" max="9" width="11.5"/>
+    <col min="10" max="10" width="13.875" customWidth="1"/>
+    <col min="12" max="12" width="16.875" customWidth="1"/>
+    <col min="22" max="22" width="13.625" customWidth="1"/>
+    <col min="24" max="26" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2745,9 +2871,175 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13">
+        <v>8585656999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>143</v>
+      </c>
+      <c r="J13" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L13" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" t="s">
+        <v>147</v>
+      </c>
+      <c r="N13">
+        <v>400001</v>
+      </c>
+      <c r="O13" t="s">
+        <v>148</v>
+      </c>
+      <c r="P13" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>150</v>
+      </c>
+      <c r="R13" t="s">
+        <v>151</v>
+      </c>
+      <c r="S13" t="s">
+        <v>152</v>
+      </c>
+      <c r="T13" t="s">
+        <v>153</v>
+      </c>
+      <c r="U13" t="s">
+        <v>154</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="W13" t="s">
+        <v>156</v>
+      </c>
+      <c r="X13">
+        <v>7874563215</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:1">
+      <c r="A15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16">
+        <v>8585656999</v>
+      </c>
+      <c r="K16" t="s">
+        <v>143</v>
+      </c>
+      <c r="L16" t="s">
+        <v>144</v>
+      </c>
+      <c r="M16" t="s">
+        <v>145</v>
+      </c>
+      <c r="N16" t="s">
+        <v>146</v>
+      </c>
+      <c r="O16" t="s">
+        <v>147</v>
+      </c>
+      <c r="P16">
+        <v>400001</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>148</v>
+      </c>
+      <c r="R16" t="s">
+        <v>149</v>
+      </c>
+      <c r="S16" t="s">
+        <v>150</v>
+      </c>
+      <c r="T16" t="s">
+        <v>151</v>
+      </c>
+      <c r="U16" t="s">
+        <v>152</v>
+      </c>
+      <c r="V16" t="s">
+        <v>153</v>
+      </c>
+      <c r="W16" t="s">
+        <v>154</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z16">
+        <v>7874563215</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="admin@1234"/>
+    <hyperlink ref="V13" r:id="rId2" display="abc12356@abc.com" tooltip="mailto:abc12356@abc.com"/>
+    <hyperlink ref="X16" r:id="rId2" display="abc12356@abc.com" tooltip="mailto:abc12356@abc.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Random Generation of Variable
</commit_message>
<xml_diff>
--- a/src/main/java/SOR_resources/Test_Data.xlsx
+++ b/src/main/java/SOR_resources/Test_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="181">
   <si>
     <t>Module</t>
   </si>
@@ -442,19 +442,19 @@
     <t>BC_Name</t>
   </si>
   <si>
-    <t>MaximusInfoNew</t>
+    <t>PriyaJohn</t>
   </si>
   <si>
     <t>PanNo</t>
   </si>
   <si>
-    <t>QXOPC5696Y</t>
+    <t>ZXOPC5696U</t>
   </si>
   <si>
     <t>AddharNO</t>
   </si>
   <si>
-    <t>502081483187</t>
+    <t>502081483165</t>
   </si>
   <si>
     <t>AccountNo</t>
@@ -496,7 +496,7 @@
     <t>EmailID</t>
   </si>
   <si>
-    <t>abc12356@abc.com</t>
+    <t>pqrs321@abc.com</t>
   </si>
   <si>
     <t>ContactNo</t>
@@ -508,23 +508,84 @@
     <t>AGG_Name</t>
   </si>
   <si>
+    <t>MaximusOne</t>
+  </si>
+  <si>
     <t>Qualification</t>
   </si>
   <si>
     <t>12th</t>
+  </si>
+  <si>
+    <t>Agent_Registration</t>
+  </si>
+  <si>
+    <t>Agent_Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>DateFormat</t>
+  </si>
+  <si>
+    <t>Device_Code</t>
+  </si>
+  <si>
+    <t>ABC124</t>
+  </si>
+  <si>
+    <t>Populaor_GRp</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Agent_Code</t>
+  </si>
+  <si>
+    <t>ABC457</t>
+  </si>
+  <si>
+    <t>Terminal_ID</t>
+  </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>Lattitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>SaraAlice</t>
+  </si>
+  <si>
+    <t>RajJohn</t>
+  </si>
+  <si>
+    <t>AlexEmma</t>
+  </si>
+  <si>
+    <t>JohnEmma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +597,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1010,134 +1079,134 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1146,26 +1215,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1516,279 +1587,279 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.1083333333333" customWidth="1"/>
-    <col min="4" max="4" width="25.2166666666667" customWidth="1"/>
-    <col min="5" max="5" width="21.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="33.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="13.5583333333333" customWidth="1"/>
-    <col min="8" max="8" width="20.5583333333333" customWidth="1"/>
-    <col min="9" max="9" width="14.1083333333333" customWidth="1"/>
-    <col min="10" max="10" width="12.8833333333333" customWidth="1"/>
-    <col min="11" max="11" width="15.1083333333333" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="15.3333333333333" customWidth="1"/>
-    <col min="15" max="15" width="29.5583333333333" customWidth="1"/>
-    <col min="17" max="17" width="30.5583333333333" customWidth="1"/>
-    <col min="19" max="19" width="15.1083333333333" customWidth="1"/>
-    <col min="20" max="20" width="15.3333333333333" customWidth="1"/>
-    <col min="21" max="21" width="15.1083333333333" customWidth="1"/>
-    <col min="22" max="22" width="26" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.0"/>
+    <col min="3" max="3" customWidth="true" width="15.1083333333333"/>
+    <col min="4" max="4" customWidth="true" width="25.2166666666667"/>
+    <col min="5" max="5" customWidth="true" width="21.3333333333333"/>
+    <col min="6" max="6" customWidth="true" width="33.6666666666667"/>
+    <col min="7" max="7" customWidth="true" width="13.5583333333333"/>
+    <col min="8" max="8" customWidth="true" width="20.5583333333333"/>
+    <col min="9" max="9" customWidth="true" width="14.1083333333333"/>
+    <col min="10" max="10" customWidth="true" width="12.8833333333333"/>
+    <col min="11" max="11" customWidth="true" width="15.1083333333333"/>
+    <col min="12" max="12" customWidth="true" width="26.0"/>
+    <col min="13" max="13" customWidth="true" width="11.0"/>
+    <col min="14" max="14" customWidth="true" width="15.3333333333333"/>
+    <col min="15" max="15" customWidth="true" width="29.5583333333333"/>
+    <col min="17" max="17" customWidth="true" width="30.5583333333333"/>
+    <col min="19" max="19" customWidth="true" width="15.1083333333333"/>
+    <col min="20" max="20" customWidth="true" width="15.3333333333333"/>
+    <col min="21" max="21" customWidth="true" width="15.1083333333333"/>
+    <col min="22" max="22" customWidth="true" width="26.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:3">
-      <c r="A3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" ht="15" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:3">
-      <c r="A5" s="5"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" ht="15" spans="1:10">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:1">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" s="7" customFormat="1" ht="28.5" spans="1:6">
-      <c r="A8" s="8" t="s">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" s="9" customFormat="1" ht="28.5" spans="1:6">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1" ht="15" spans="1:1">
-      <c r="A9" s="10"/>
-    </row>
-    <row r="10" s="4" customFormat="1" ht="15" spans="1:3">
-      <c r="A10" s="10"/>
-      <c r="C10" s="11"/>
-    </row>
-    <row r="11" s="7" customFormat="1" ht="15" spans="1:18">
-      <c r="A11" s="8" t="s">
+    <row r="9" s="6" customFormat="1" ht="15" spans="1:1">
+      <c r="A9" s="12"/>
+    </row>
+    <row r="10" s="6" customFormat="1" ht="15" spans="1:3">
+      <c r="A10" s="12"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" s="9" customFormat="1" ht="15" spans="1:18">
+      <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="9">
         <v>1000</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="9">
         <v>20</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="1" ht="15" spans="1:1">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" s="7" customFormat="1" ht="28.5" spans="1:19">
-      <c r="A13" s="8" t="s">
+    <row r="12" s="9" customFormat="1" ht="15" spans="1:1">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" s="9" customFormat="1" ht="28.5" spans="1:19">
+      <c r="A13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="P13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S13" s="9"/>
-    </row>
-    <row r="14" s="7" customFormat="1"/>
-    <row r="15" s="7" customFormat="1" spans="1:8">
-      <c r="A15" s="7" t="s">
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" s="9" customFormat="1"/>
+    <row r="15" s="9" customFormat="1" spans="1:8">
+      <c r="A15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1831,638 +1902,638 @@
       </c>
     </row>
     <row r="17" spans="3:12">
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" t="s" s="0">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
     </row>
     <row r="24" spans="3:6">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" spans="3:12">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="3:12">
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:12">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:12">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="31" spans="3:10">
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="3:10">
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="3:10">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="34" spans="3:10">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="3:10">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="3:10">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="37" spans="3:10">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="3:10">
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="J38" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="39" spans="3:10">
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="3:10">
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="41" spans="3:10">
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="H41" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J41" s="7" t="s">
+      <c r="J41" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="42" spans="3:6">
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="6" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2480,7 +2551,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -2488,200 +2559,122 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.5583333333333" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.44166666666667" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.4416666666667" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.8833333333333" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.6666666666667" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.5583333333333" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.4416666666667" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.3333333333333" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.5583333333333" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13.4416666666667" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.1083333333333" style="4" customWidth="1"/>
-    <col min="12" max="18" width="13.4416666666667" style="4" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="6" width="12.5583333333333"/>
+    <col min="2" max="2" customWidth="true" style="6" width="7.44166666666667"/>
+    <col min="3" max="3" customWidth="true" style="6" width="13.4416666666667"/>
+    <col min="4" max="4" customWidth="true" style="6" width="21.8833333333333"/>
+    <col min="5" max="5" customWidth="true" style="6" width="16.6666666666667"/>
+    <col min="6" max="6" customWidth="true" style="6" width="23.5583333333333"/>
+    <col min="7" max="7" customWidth="true" style="6" width="13.4416666666667"/>
+    <col min="8" max="8" customWidth="true" style="6" width="15.3333333333333"/>
+    <col min="9" max="9" customWidth="true" style="6" width="14.5583333333333"/>
+    <col min="10" max="10" customWidth="true" style="6" width="13.4416666666667"/>
+    <col min="11" max="11" customWidth="true" style="6" width="15.1083333333333"/>
+    <col min="12" max="18" customWidth="true" style="6" width="13.4416666666667"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:18">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="15" spans="1:1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-    </row>
-    <row r="2" ht="15" spans="1:18">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" ht="42.75" spans="1:10">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="6">
         <v>15</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-    </row>
-    <row r="3" ht="15" spans="1:18">
-      <c r="A3" s="5"/>
-      <c r="B3"/>
-      <c r="C3" s="6"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-    </row>
-    <row r="4" ht="15" spans="1:18">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="3" ht="15" spans="1:3">
+      <c r="A3" s="7"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" ht="28.5" spans="1:8">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-    </row>
-    <row r="5" ht="15" spans="1:18">
-      <c r="A5" s="5"/>
-      <c r="B5"/>
-      <c r="C5" s="6"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-    </row>
-    <row r="6" ht="15" spans="1:18">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="5" ht="15" spans="1:3">
+      <c r="A5" s="7"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" ht="15" spans="1:10">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
     </row>
     <row r="9" spans="3:6">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2694,29 +2687,36 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="18.125" customWidth="1"/>
-    <col min="6" max="6" width="26.625" customWidth="1"/>
-    <col min="7" max="7" width="14.375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5"/>
+    <col min="2" max="2" customWidth="true" width="10.625"/>
+    <col min="3" max="3" customWidth="true" width="12.5"/>
+    <col min="4" max="4" customWidth="true" width="18.625"/>
+    <col min="5" max="5" customWidth="true" width="18.125"/>
+    <col min="6" max="6" customWidth="true" width="26.625"/>
+    <col min="7" max="7" customWidth="true" width="14.375"/>
     <col min="8" max="9" width="11.5"/>
-    <col min="10" max="10" width="13.875" customWidth="1"/>
-    <col min="12" max="12" width="16.875" customWidth="1"/>
-    <col min="22" max="22" width="13.625" customWidth="1"/>
-    <col min="24" max="26" width="11.5"/>
+    <col min="10" max="10" customWidth="true" width="13.875"/>
+    <col min="11" max="11" width="11.5"/>
+    <col min="12" max="12" customWidth="true" width="16.875"/>
+    <col min="14" max="14" customWidth="true" width="16.875"/>
+    <col min="15" max="15" customWidth="true" width="12.625"/>
+    <col min="22" max="22" customWidth="true" width="13.625"/>
+    <col min="24" max="32" width="11.5"/>
+    <col min="34" max="34" width="11.5"/>
+    <col min="36" max="36" width="11.5"/>
+    <col min="38" max="38" width="11.5"/>
+    <col min="40" max="40" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:40">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -2753,101 +2753,143 @@
       <c r="L1" s="1">
         <v>11</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="0">
         <v>12</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="0">
         <v>13</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="0">
         <v>14</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="0">
         <v>15</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="0">
         <v>16</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="0">
         <v>17</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="0">
         <v>18</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="0">
         <v>19</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="0">
         <v>20</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="0">
         <v>21</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="0">
         <v>22</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="0">
         <v>23</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="0">
         <v>24</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="0">
         <v>25</v>
       </c>
+      <c r="AA1" s="0">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="0">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="0">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="0">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="0">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="0">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="0">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="0">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="0">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>131</v>
       </c>
     </row>
@@ -2872,174 +2914,302 @@
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="B13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="C13" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>8585656999</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="0">
         <v>400001</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="V13" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="X13">
-        <v>7874563215</v>
+      <c r="X13" s="0">
+        <v>9874563215</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:1">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="B16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="C16" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="J16" s="0">
+        <v>8585656999</v>
+      </c>
+      <c r="K16" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="L16" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="M16" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="N16" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="O16" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="P16" s="0">
+        <v>400001</v>
+      </c>
+      <c r="Q16" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="R16" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="S16" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="T16" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="U16" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="V16" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="W16" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y16" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="Z16" s="0">
+        <v>9874563215</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" spans="1:1">
+      <c r="A18" t="s" s="0">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40">
+      <c r="A19" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="B19" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="H16" t="s">
-        <v>160</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="C19" t="s" s="0">
+        <v>164</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="J19" s="4">
+        <v>30856</v>
+      </c>
+      <c r="K19" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="J16">
+      <c r="L19" s="0">
         <v>8585656999</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M19" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N19" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O19" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="P19" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="Q19" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="R19" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="S19" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="T19" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="U19" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="V19" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="W19" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="X19" s="0">
+        <v>10.32</v>
+      </c>
+      <c r="Y19" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="Z19" s="0">
+        <v>11.33</v>
+      </c>
+      <c r="AA19" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="N16" t="s">
+      <c r="AB19" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="O16" t="s">
+      <c r="AC19" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="P16">
+      <c r="AD19" s="0">
         <v>400001</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="AE19" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="R16" t="s">
+      <c r="AF19" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="S16" t="s">
+      <c r="AG19" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="T16" t="s">
+      <c r="AH19" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="U16" t="s">
+      <c r="AI19" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="V16" t="s">
+      <c r="AJ19" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="W16" t="s">
+      <c r="AK19" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="AL19" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AM19" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="Z16">
-        <v>7874563215</v>
+      <c r="AN19" s="0">
+        <v>9874563215</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="admin@1234"/>
-    <hyperlink ref="V13" r:id="rId2" display="abc12356@abc.com" tooltip="mailto:abc12356@abc.com"/>
-    <hyperlink ref="X16" r:id="rId2" display="abc12356@abc.com" tooltip="mailto:abc12356@abc.com"/>
+    <hyperlink ref="V13" r:id="rId2" display="pqrs321@abc.com" tooltip="mailto:pqrs321@abc.com"/>
+    <hyperlink ref="X16" r:id="rId2" display="pqrs321@abc.com" tooltip="mailto:pqrs321@abc.com"/>
+    <hyperlink ref="AL19" r:id="rId2" display="pqrs321@abc.com" tooltip="mailto:pqrs321@abc.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Agent Add verify done
</commit_message>
<xml_diff>
--- a/src/main/java/SOR_resources/Test_Data.xlsx
+++ b/src/main/java/SOR_resources/Test_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="221">
   <si>
     <t>Module</t>
   </si>
@@ -415,7 +415,7 @@
     <t>Grp_Name</t>
   </si>
   <si>
-    <t>Automation</t>
+    <t>SaraPriya</t>
   </si>
   <si>
     <t>Grp_Desc</t>
@@ -430,6 +430,9 @@
     <t>Switch_name</t>
   </si>
   <si>
+    <t>EmmaPriya</t>
+  </si>
+  <si>
     <t>Switch_Desc</t>
   </si>
   <si>
@@ -442,136 +445,253 @@
     <t>BC_Name</t>
   </si>
   <si>
+    <t>AliceEmma</t>
+  </si>
+  <si>
+    <t>PanNo</t>
+  </si>
+  <si>
+    <t>ZXOPC5696U</t>
+  </si>
+  <si>
+    <t>AddharNO</t>
+  </si>
+  <si>
+    <t>502081483165</t>
+  </si>
+  <si>
+    <t>AccountNo</t>
+  </si>
+  <si>
+    <t>IFSCcode</t>
+  </si>
+  <si>
+    <t>HDFC0000967</t>
+  </si>
+  <si>
+    <t>Addess</t>
+  </si>
+  <si>
+    <t>Thane Maharshtra</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Sangli</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Satna</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>pqrs321@abc.com</t>
+  </si>
+  <si>
+    <t>ContactNo</t>
+  </si>
+  <si>
+    <t>AGG_Registration</t>
+  </si>
+  <si>
+    <t>AGG_Name</t>
+  </si>
+  <si>
+    <t>AlicePriya</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>Agent_Registration</t>
+  </si>
+  <si>
+    <t>Agent_Name</t>
+  </si>
+  <si>
+    <t>JohnPriya</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>DateFormat</t>
+  </si>
+  <si>
+    <t>23-06-1984</t>
+  </si>
+  <si>
+    <t>Device_Code</t>
+  </si>
+  <si>
+    <t>ABC124</t>
+  </si>
+  <si>
+    <t>Populaor_GRp</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Agent_Code</t>
+  </si>
+  <si>
+    <t>ABC457</t>
+  </si>
+  <si>
+    <t>Terminal_ID</t>
+  </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>Lattitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>SaraRaj</t>
+  </si>
+  <si>
+    <t>SaraEmma</t>
+  </si>
+  <si>
+    <t>JohnEmma</t>
+  </si>
+  <si>
+    <t>BobBob</t>
+  </si>
+  <si>
+    <t>AlexBob</t>
+  </si>
+  <si>
+    <t>PriyaPriya</t>
+  </si>
+  <si>
+    <t>AlexSara</t>
+  </si>
+  <si>
+    <t>JohnSara</t>
+  </si>
+  <si>
+    <t>PriyaAlice</t>
+  </si>
+  <si>
+    <t>JohnAlex</t>
+  </si>
+  <si>
+    <t>EmmaEmma</t>
+  </si>
+  <si>
+    <t>RajEmma</t>
+  </si>
+  <si>
+    <t>AliceAlice</t>
+  </si>
+  <si>
+    <t>RajJohn</t>
+  </si>
+  <si>
+    <t>BobRaj</t>
+  </si>
+  <si>
+    <t>AlexEmma</t>
+  </si>
+  <si>
+    <t>BobJohn</t>
+  </si>
+  <si>
+    <t>SaraAlex</t>
+  </si>
+  <si>
+    <t>SaraBob</t>
+  </si>
+  <si>
+    <t>BobAlice</t>
+  </si>
+  <si>
+    <t>EmmaAlex</t>
+  </si>
+  <si>
+    <t>EmmaSara</t>
+  </si>
+  <si>
+    <t>JohnAlice</t>
+  </si>
+  <si>
+    <t>EmmaBob</t>
+  </si>
+  <si>
+    <t>AliceRaj</t>
+  </si>
+  <si>
+    <t>RajAlice</t>
+  </si>
+  <si>
+    <t>BobAlex</t>
+  </si>
+  <si>
+    <t>PriyaRaj</t>
+  </si>
+  <si>
+    <t>RajRaj</t>
+  </si>
+  <si>
+    <t>PriyaBob</t>
+  </si>
+  <si>
+    <t>AliceJohn</t>
+  </si>
+  <si>
+    <t>AliceAlex</t>
+  </si>
+  <si>
+    <t>BobEmma</t>
+  </si>
+  <si>
+    <t>RajSara</t>
+  </si>
+  <si>
+    <t>RajPriya</t>
+  </si>
+  <si>
     <t>PriyaJohn</t>
   </si>
   <si>
-    <t>PanNo</t>
-  </si>
-  <si>
-    <t>ZXOPC5696U</t>
-  </si>
-  <si>
-    <t>AddharNO</t>
-  </si>
-  <si>
-    <t>502081483165</t>
-  </si>
-  <si>
-    <t>AccountNo</t>
-  </si>
-  <si>
-    <t>IFSCcode</t>
-  </si>
-  <si>
-    <t>HDFC0000967</t>
-  </si>
-  <si>
-    <t>Addess</t>
-  </si>
-  <si>
-    <t>Thane Maharshtra</t>
-  </si>
-  <si>
-    <t>PinCode</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Sangli</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Satna</t>
-  </si>
-  <si>
-    <t>EmailID</t>
-  </si>
-  <si>
-    <t>pqrs321@abc.com</t>
-  </si>
-  <si>
-    <t>ContactNo</t>
-  </si>
-  <si>
-    <t>AGG_Registration</t>
-  </si>
-  <si>
-    <t>AGG_Name</t>
-  </si>
-  <si>
-    <t>MaximusOne</t>
-  </si>
-  <si>
-    <t>Qualification</t>
-  </si>
-  <si>
-    <t>12th</t>
-  </si>
-  <si>
-    <t>Agent_Registration</t>
-  </si>
-  <si>
-    <t>Agent_Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>DateFormat</t>
-  </si>
-  <si>
-    <t>Device_Code</t>
-  </si>
-  <si>
-    <t>ABC124</t>
-  </si>
-  <si>
-    <t>Populaor_GRp</t>
-  </si>
-  <si>
-    <t>Rural</t>
-  </si>
-  <si>
-    <t>Agent_Code</t>
-  </si>
-  <si>
-    <t>ABC457</t>
-  </si>
-  <si>
-    <t>Terminal_ID</t>
-  </si>
-  <si>
-    <t>T02</t>
-  </si>
-  <si>
-    <t>Lattitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
+    <t>RajBob</t>
+  </si>
+  <si>
+    <t>PriyaEmma</t>
+  </si>
+  <si>
+    <t>AlexAlice</t>
   </si>
   <si>
     <t>SaraAlice</t>
   </si>
   <si>
-    <t>RajJohn</t>
-  </si>
-  <si>
-    <t>AlexEmma</t>
-  </si>
-  <si>
-    <t>JohnEmma</t>
+    <t>EmmaJohn</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1326,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1240,6 +1360,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2690,7 +2811,7 @@
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2879,7 +3000,7 @@
         <v>127</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>129</v>
@@ -2897,17 +3018,17 @@
       <c r="A10" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>128</v>
+      <c r="B10" t="s" s="0">
+        <v>202</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F10" s="3">
         <v>20</v>
@@ -2915,78 +3036,78 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s" s="0">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H13" s="0">
         <v>8585656999</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J13" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L13" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M13" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N13" s="0">
         <v>400001</v>
       </c>
       <c r="O13" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P13" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q13" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R13" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S13" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T13" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="U13" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="W13" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="X13" s="0">
         <v>9874563215</v>
@@ -2994,84 +3115,84 @@
     </row>
     <row r="15" customFormat="1" spans="1:1">
       <c r="A15" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J16" s="0">
         <v>8585656999</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L16" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M16" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N16" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O16" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P16" s="0">
         <v>400001</v>
       </c>
       <c r="Q16" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R16" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="S16" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="T16" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U16" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V16" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="W16" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Y16" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Z16" s="0">
         <v>9874563215</v>
@@ -3079,126 +3200,126 @@
     </row>
     <row r="18" customFormat="1" spans="1:1">
       <c r="A18" t="s" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:40">
       <c r="A19" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>166</v>
-      </c>
-      <c r="J19" s="4">
-        <v>30856</v>
+        <v>168</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L19" s="0">
         <v>8585656999</v>
       </c>
       <c r="M19" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N19" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="O19" t="s" s="0">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P19" t="s" s="0">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="Q19" t="s" s="0">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="R19" t="s" s="0">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="S19" t="s" s="0">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="T19" t="s" s="0">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="U19" t="s" s="0">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="V19" t="s" s="0">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="W19" t="s" s="0">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="X19" s="0">
         <v>10.32</v>
       </c>
       <c r="Y19" t="s" s="0">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="Z19" s="0">
         <v>11.33</v>
       </c>
       <c r="AA19" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AB19" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AC19" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AD19" s="0">
         <v>400001</v>
       </c>
       <c r="AE19" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AF19" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AG19" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AH19" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AI19" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AJ19" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AK19" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM19" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AN19" s="0">
         <v>9874563215</v>

</xml_diff>

<commit_message>
Chnages Till 07/11/2024 12:22
</commit_message>
<xml_diff>
--- a/src/main/java/SOR_resources/Test_Data.xlsx
+++ b/src/main/java/SOR_resources/Test_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="232">
   <si>
     <t>Module</t>
   </si>
@@ -692,6 +692,39 @@
   </si>
   <si>
     <t>EmmaJohn</t>
+  </si>
+  <si>
+    <t>AliceBob</t>
+  </si>
+  <si>
+    <t>AlexAlex</t>
+  </si>
+  <si>
+    <t>JohnBob</t>
+  </si>
+  <si>
+    <t>JohnRaj</t>
+  </si>
+  <si>
+    <t>AlexJohn</t>
+  </si>
+  <si>
+    <t>EmmaAlice</t>
+  </si>
+  <si>
+    <t>BobPriya</t>
+  </si>
+  <si>
+    <t>PriyaSara</t>
+  </si>
+  <si>
+    <t>AliceSara</t>
+  </si>
+  <si>
+    <t>PriyaAlex</t>
+  </si>
+  <si>
+    <t>SaraJohn</t>
   </si>
 </sst>
 </file>
@@ -3000,7 +3033,7 @@
         <v>127</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>129</v>
@@ -3019,7 +3052,7 @@
         <v>132</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>134</v>
@@ -3044,7 +3077,7 @@
         <v>137</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>139</v>
@@ -3123,7 +3156,7 @@
         <v>159</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>139</v>
@@ -3208,7 +3241,7 @@
         <v>164</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>166</v>

</xml_diff>

<commit_message>
Major Chnages in Code
</commit_message>
<xml_diff>
--- a/src/main/java/SOR_resources/Test_Data.xlsx
+++ b/src/main/java/SOR_resources/Test_Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="263">
   <si>
     <t>Module</t>
   </si>
@@ -395,7 +395,7 @@
     <t>Login Page</t>
   </si>
   <si>
-    <t>http://localhost:8065/Login.aspx</t>
+    <t>http://localhost:8066/Login.aspx</t>
   </si>
   <si>
     <t>Maximus</t>
@@ -419,7 +419,7 @@
     <t>Grp_Name</t>
   </si>
   <si>
-    <t>BobBob</t>
+    <t>QuicksunTechnologiesPvtLtd</t>
   </si>
   <si>
     <t>Grp_Desc</t>
@@ -434,6 +434,9 @@
     <t>Switch_name</t>
   </si>
   <si>
+    <t>Vakrangi</t>
+  </si>
+  <si>
     <t>Switch_Desc</t>
   </si>
   <si>
@@ -446,7 +449,7 @@
     <t>BC_Name</t>
   </si>
   <si>
-    <t>AlexPriya</t>
+    <t>Spicemoney</t>
   </si>
   <si>
     <t>PanNo</t>
@@ -512,7 +515,7 @@
     <t>AGG_Name</t>
   </si>
   <si>
-    <t>BobAlex</t>
+    <t>Mobileware</t>
   </si>
   <si>
     <t>Qualification</t>
@@ -527,7 +530,7 @@
     <t>Agent_Name</t>
   </si>
   <si>
-    <t>EmmaSara</t>
+    <t>MuthootFincorpLtd</t>
   </si>
   <si>
     <t>Gender</t>
@@ -575,109 +578,247 @@
     <t>Create User</t>
   </si>
   <si>
-    <t>EgDtmMyycV9dHAO</t>
-  </si>
-  <si>
-    <t>AliceAlex</t>
-  </si>
-  <si>
-    <t>RajPriya</t>
-  </si>
-  <si>
-    <t>AlexAlex</t>
-  </si>
-  <si>
-    <t>AlexJohn</t>
-  </si>
-  <si>
-    <t>SaraBob</t>
-  </si>
-  <si>
-    <t>SaraAlice</t>
-  </si>
-  <si>
-    <t>AliceAlice</t>
-  </si>
-  <si>
-    <t>AlexEmma</t>
-  </si>
-  <si>
-    <t>SaraPriya</t>
-  </si>
-  <si>
-    <t>AliceSara</t>
-  </si>
-  <si>
-    <t>AlexSara</t>
-  </si>
-  <si>
-    <t>RajAlice</t>
-  </si>
-  <si>
-    <t>EmmaJohn</t>
-  </si>
-  <si>
-    <t>AlicePriya</t>
-  </si>
-  <si>
-    <t>PriyaRaj</t>
-  </si>
-  <si>
-    <t>JohnBob</t>
-  </si>
-  <si>
-    <t>EmmaRaj</t>
-  </si>
-  <si>
-    <t>PriyaAlex</t>
-  </si>
-  <si>
-    <t>JohnRaj</t>
-  </si>
-  <si>
-    <t>SaraEmma</t>
-  </si>
-  <si>
-    <t>SaraSara</t>
-  </si>
-  <si>
-    <t>AlexAlice</t>
-  </si>
-  <si>
-    <t>PriyaBob</t>
-  </si>
-  <si>
-    <t>EmmaAlex</t>
-  </si>
-  <si>
-    <t>BobSara</t>
-  </si>
-  <si>
-    <t>RajJohn</t>
-  </si>
-  <si>
-    <t>AliceJohn</t>
-  </si>
-  <si>
-    <t>RajEmma</t>
-  </si>
-  <si>
-    <t>RajRaj</t>
-  </si>
-  <si>
-    <t>BobAlice</t>
-  </si>
-  <si>
-    <t>AlexBob</t>
+    <t>jOP8zJcP</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Admin Management</t>
+  </si>
+  <si>
+    <t>Rule Management</t>
+  </si>
+  <si>
+    <t>BC Management</t>
+  </si>
+  <si>
+    <t>Aggregator Management</t>
+  </si>
+  <si>
+    <t>Agent Management</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Application Management</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Tester_5108</t>
+  </si>
+  <si>
+    <t>Designer_7733</t>
+  </si>
+  <si>
+    <t>Analyst_9054</t>
+  </si>
+  <si>
+    <t>Tester_3231</t>
+  </si>
+  <si>
+    <t>Admin_1339</t>
+  </si>
+  <si>
+    <t>User_8463</t>
+  </si>
+  <si>
+    <t>Analyst9421</t>
+  </si>
+  <si>
+    <t>Manager1600</t>
+  </si>
+  <si>
+    <t>Tester9709</t>
+  </si>
+  <si>
+    <t>Developer5921</t>
+  </si>
+  <si>
+    <t>Developer2055</t>
+  </si>
+  <si>
+    <t>Admin2238</t>
+  </si>
+  <si>
+    <t>Admin2687</t>
+  </si>
+  <si>
+    <t>Analyst5679</t>
+  </si>
+  <si>
+    <t>Analyst8386</t>
+  </si>
+  <si>
+    <t>User7258</t>
+  </si>
+  <si>
+    <t>Designer2855</t>
+  </si>
+  <si>
+    <t>Designer9730</t>
+  </si>
+  <si>
+    <t>Developer6483</t>
+  </si>
+  <si>
+    <t>Manager2414</t>
+  </si>
+  <si>
+    <t>Manager6334</t>
+  </si>
+  <si>
+    <t>Manager8260</t>
+  </si>
+  <si>
+    <t>Developer5782</t>
+  </si>
+  <si>
+    <t>Manager4769</t>
+  </si>
+  <si>
+    <t>Analyst6540</t>
+  </si>
+  <si>
+    <t>User3654</t>
+  </si>
+  <si>
+    <t>Manager1117</t>
+  </si>
+  <si>
+    <t>Analyst7563</t>
+  </si>
+  <si>
+    <t>Admin5252</t>
+  </si>
+  <si>
+    <t>QFdsGPMzjN</t>
+  </si>
+  <si>
+    <t>UG8TH9SDGkpxVgW</t>
+  </si>
+  <si>
+    <t>qrmhNZSOY7eP</t>
+  </si>
+  <si>
+    <t>lSpEGAF95bU</t>
+  </si>
+  <si>
+    <t>Designer7083</t>
+  </si>
+  <si>
+    <t>vQD32kX2Ta</t>
+  </si>
+  <si>
+    <t>User4942</t>
+  </si>
+  <si>
+    <t>tgZ7ol</t>
+  </si>
+  <si>
+    <t>User3441</t>
+  </si>
+  <si>
+    <t>UcnPH8etZIR</t>
+  </si>
+  <si>
+    <t>Tester5830</t>
+  </si>
+  <si>
+    <t>He63YVwd</t>
+  </si>
+  <si>
+    <t>Developer7615</t>
+  </si>
+  <si>
+    <t>User7248</t>
+  </si>
+  <si>
+    <t>Tester7828</t>
+  </si>
+  <si>
+    <t>Mml9uQW5hr007K</t>
+  </si>
+  <si>
+    <t>Manager9325</t>
+  </si>
+  <si>
+    <t>CZoLdfPe9Ao5bx2</t>
+  </si>
+  <si>
+    <t>Designer5037</t>
+  </si>
+  <si>
+    <t>h9vxFK</t>
+  </si>
+  <si>
+    <t>Developer7621</t>
+  </si>
+  <si>
+    <t>4pvMxY</t>
+  </si>
+  <si>
+    <t>Tester8746</t>
+  </si>
+  <si>
+    <t>ODDKeGxBz7VN</t>
+  </si>
+  <si>
+    <t>Tester9850</t>
+  </si>
+  <si>
+    <t>Designer4590</t>
+  </si>
+  <si>
+    <t>vHrXNlL9nPii3</t>
+  </si>
+  <si>
+    <t>Designer8511</t>
+  </si>
+  <si>
+    <t>Designer9020</t>
+  </si>
+  <si>
+    <t>Accupaydtech</t>
+  </si>
+  <si>
+    <t>Admin8414</t>
+  </si>
+  <si>
+    <t>Developer2434</t>
+  </si>
+  <si>
+    <t>M2WmH9Z3OkvI</t>
+  </si>
+  <si>
+    <t>Designer1510</t>
+  </si>
+  <si>
+    <t>Manager9424</t>
+  </si>
+  <si>
+    <t>Developer5449</t>
+  </si>
+  <si>
+    <t>Manager1798</t>
+  </si>
+  <si>
+    <t>User7622</t>
+  </si>
+  <si>
+    <t>KYifyxM4zTY4z8</t>
   </si>
   <si>
     <t>Rapipay</t>
-  </si>
-  <si>
-    <t>Savatra</t>
-  </si>
-  <si>
-    <t>Muthoot Fincorp Ltd</t>
   </si>
 </sst>
 </file>
@@ -2794,16 +2935,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AN22"/>
+  <dimension ref="A1:AN34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A13" sqref="$A13:$XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="17.5"/>
-    <col min="2" max="2" customWidth="true" width="10.625"/>
+    <col min="2" max="2" customWidth="true" width="26.875"/>
     <col min="3" max="3" customWidth="true" width="12.5"/>
     <col min="4" max="4" customWidth="true" width="18.625"/>
     <col min="5" max="5" customWidth="true" width="18.125"/>
@@ -2951,7 +3092,7 @@
       </c>
     </row>
     <row r="3" spans="6:6">
-      <c r="F3" t="s" s="0">
+      <c r="F3" s="2" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2991,7 +3132,7 @@
         <v>128</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>130</v>
@@ -3010,16 +3151,16 @@
         <v>133</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>214</v>
+        <v>134</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>131</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F10" s="3">
         <v>20</v>
@@ -3027,78 +3168,78 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s" s="0">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H13" s="0">
         <v>8585656999</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J13" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L13" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M13" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N13" s="0">
         <v>400001</v>
       </c>
       <c r="O13" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P13" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Q13" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R13" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="S13" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="T13" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="U13" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="W13" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X13" s="0">
         <v>9874563215</v>
@@ -3106,84 +3247,84 @@
     </row>
     <row r="15" customFormat="1" spans="1:1">
       <c r="A15" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" t="s" s="0">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J16" s="0">
         <v>8585656999</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L16" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M16" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N16" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O16" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P16" s="0">
         <v>400001</v>
       </c>
       <c r="Q16" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="R16" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="S16" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T16" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="U16" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V16" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="W16" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Y16" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Z16" s="0">
         <v>9874563215</v>
@@ -3191,126 +3332,126 @@
     </row>
     <row r="18" customFormat="1" spans="1:1">
       <c r="A18" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:40">
       <c r="A19" t="s" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>212</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L19" s="0">
         <v>8585656999</v>
       </c>
       <c r="M19" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N19" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O19" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P19" t="s" s="0">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q19" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="R19" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S19" t="s" s="0">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T19" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="U19" t="s" s="0">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="V19" t="s" s="0">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="W19" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="X19" s="0">
         <v>10.32</v>
       </c>
       <c r="Y19" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Z19" s="0">
         <v>11.33</v>
       </c>
       <c r="AA19" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AB19" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AC19" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AD19" s="0">
         <v>400001</v>
       </c>
       <c r="AE19" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AF19" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG19" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AH19" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AI19" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AJ19" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AK19" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AM19" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AN19" s="0">
         <v>9874563215</v>
@@ -3318,7 +3459,7 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s" s="0">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3326,13 +3467,93 @@
         <v>16</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>181</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s" s="0">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="J28" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="K28" t="s" s="0">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s" s="0">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s" s="0">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s" s="0">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s" s="0">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s" s="0">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3342,6 +3563,7 @@
     <hyperlink ref="X16" r:id="rId2" display="pqrs321@abc.com" tooltip="mailto:pqrs321@abc.com"/>
     <hyperlink ref="AL19" r:id="rId2" display="pqrs321@abc.com" tooltip="mailto:pqrs321@abc.com"/>
     <hyperlink ref="D22" r:id="rId1" display="admin@1234"/>
+    <hyperlink ref="F3" r:id="rId3" display="http://localhost:8066/Login.aspx"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>